<commit_message>
Add connectivity matrix and update results
</commit_message>
<xml_diff>
--- a/current_population.xlsx
+++ b/current_population.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -246,9 +246,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>